<commit_message>
fix timmy formatting of maps
</commit_message>
<xml_diff>
--- a/timesheet.xlsx
+++ b/timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\video-typer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBE6738-02E0-47C0-8757-3B13EAE7F9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09485AF4-875A-4019-BDA7-8472FB87151E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>Start</t>
   </si>
@@ -73,16 +73,29 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Potential $</t>
+    <t>we didn’t go</t>
+  </si>
+  <si>
+    <t>this way</t>
+  </si>
+  <si>
+    <t>^ How we're actually gonna split it I guess?</t>
+  </si>
+  <si>
+    <t>$ per hour</t>
+  </si>
+  <si>
+    <t>original split plan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -121,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -129,6 +142,7 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -238,10 +252,10 @@
             <c:numRef>
               <c:f>Sheet1!$G$3</c:f>
               <c:numCache>
-                <c:formatCode>[$-F400]h:mm:ss\ AM/PM</c:formatCode>
+                <c:formatCode>[h]:mm:ss;@</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.98263888888888884</c:v>
+                  <c:v>1.7173611111111109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -337,7 +351,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="[$-F400]h:mm:ss\ AM/PM" sourceLinked="1"/>
+        <c:numFmt formatCode="[h]:mm:ss;@" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4084,10 +4098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4100,9 +4114,10 @@
     <col min="12" max="12" width="10.140625" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
     <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4116,10 +4131,13 @@
         <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4150,14 +4168,21 @@
       </c>
       <c r="M2" s="3">
         <f>L2/$L$4</f>
-        <v>0.41451909881365012</v>
+        <v>0.28830777642868577</v>
       </c>
       <c r="N2" s="5">
         <f>$N$4*M2</f>
-        <v>829.03819762730029</v>
+        <v>576.61555285737154</v>
+      </c>
+      <c r="P2" s="5">
+        <v>1000</v>
+      </c>
+      <c r="Q2" s="5">
+        <f>P2/(L2*24)</f>
+        <v>59.891197657812349</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44487.838217592594</v>
       </c>
@@ -4170,8 +4195,8 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="2">
-        <v>0.98263888888888884</v>
+      <c r="G3" s="7">
+        <v>1.7173611111111109</v>
       </c>
       <c r="I3" t="s">
         <v>5</v>
@@ -4179,20 +4204,27 @@
       <c r="K3" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="7">
         <f>SUM(G:G)</f>
-        <v>0.98263888888888884</v>
+        <v>1.7173611111111109</v>
       </c>
       <c r="M3" s="3">
         <f>L3/$L$4</f>
-        <v>0.58548090118634988</v>
+        <v>0.71169222357131423</v>
       </c>
       <c r="N3" s="5">
         <f>$N$4*M3</f>
-        <v>1170.9618023726998</v>
+        <v>1423.3844471426285</v>
+      </c>
+      <c r="P3" s="5">
+        <v>1000</v>
+      </c>
+      <c r="Q3" s="5">
+        <f>P3/(L3*24)</f>
+        <v>24.262029923170243</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44487.914756944447</v>
       </c>
@@ -4214,14 +4246,14 @@
       </c>
       <c r="L4" s="6">
         <f>SUM(L2:L3)</f>
-        <v>1.6783449074048096</v>
+        <v>2.4130671296270316</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="5">
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44488.318136574075</v>
       </c>
@@ -4239,8 +4271,11 @@
         <v>5</v>
       </c>
       <c r="N5" s="5"/>
+      <c r="P5" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44488.913645833331</v>
       </c>
@@ -4257,8 +4292,11 @@
       <c r="I6" t="s">
         <v>5</v>
       </c>
+      <c r="N6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44488.938252314816</v>
       </c>
@@ -4275,8 +4313,11 @@
       <c r="I7" t="s">
         <v>5</v>
       </c>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44489.489594907405</v>
       </c>
@@ -4293,7 +4334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44489.656793981485</v>
       </c>
@@ -4305,7 +4346,7 @@
         <v>5.9884259258979E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44490.840902777774</v>
       </c>
@@ -4317,7 +4358,7 @@
         <v>5.0925925927003846E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44490.923622685186</v>
       </c>
@@ -4329,7 +4370,7 @@
         <v>2.0925925928167999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44490.946701388886</v>
       </c>
@@ -4341,7 +4382,7 @@
         <v>4.5370370426098816E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44491.340740740743</v>
       </c>
@@ -4353,7 +4394,7 @@
         <v>5.0613425926712807E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44491.389224537037</v>
       </c>
@@ -4365,7 +4406,7 @@
         <v>1.7731481479131617E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44491.473657407405</v>
       </c>
@@ -4377,7 +4418,7 @@
         <v>3.1412037038535345E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44491.548900462964</v>
       </c>

</xml_diff>